<commit_message>
Added new contact code
</commit_message>
<xml_diff>
--- a/src/main/java/com/qa/hs/keyword/scenarios/hubspot_scenarios.xlsx
+++ b/src/main/java/com/qa/hs/keyword/scenarios/hubspot_scenarios.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1024812\Desktop\Selenium\KeywordDrivenFramework\src\main\java\com\qa\hs\keyword\scenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BCD710E-FE84-40CE-AC72-B340725F1B83}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00B9856D-3D64-4A29-A7A2-D905E2DDBD9D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="60">
   <si>
     <t>action</t>
   </si>
@@ -171,6 +171,45 @@
   </si>
   <si>
     <t>Mouse Hover on Contacts</t>
+  </si>
+  <si>
+    <t>Enter Contact First Name</t>
+  </si>
+  <si>
+    <t>Enter Contact Last Name</t>
+  </si>
+  <si>
+    <t>Enter Contact Position</t>
+  </si>
+  <si>
+    <t>//input[@name='first_name' and @id='first_name']</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>//input[@name='surname' and @id='surname']</t>
+  </si>
+  <si>
+    <t>Test123</t>
+  </si>
+  <si>
+    <t>//input[@name='company_position']</t>
+  </si>
+  <si>
+    <t>Click on New Contact</t>
+  </si>
+  <si>
+    <t>//a[contains(text(),'New Contact')]</t>
+  </si>
+  <si>
+    <t>Manager</t>
+  </si>
+  <si>
+    <t>Click on Save button</t>
+  </si>
+  <si>
+    <t>//input[@type='submit' and @value='Save']</t>
   </si>
 </sst>
 </file>
@@ -841,17 +880,17 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7865F4C5-E86F-49A0-A484-4A61E21F3D70}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="23" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.58203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="43.58203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="27.9140625" bestFit="1" customWidth="1"/>
   </cols>
@@ -994,18 +1033,86 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>55</v>
       </c>
       <c r="B9" t="s">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="C9" t="s">
-        <v>5</v>
+        <v>56</v>
       </c>
       <c r="D9" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="E9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" t="s">
+        <v>50</v>
+      </c>
+      <c r="D10" t="s">
+        <v>2</v>
+      </c>
+      <c r="E10" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>48</v>
+      </c>
+      <c r="B11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" t="s">
+        <v>52</v>
+      </c>
+      <c r="D11" t="s">
+        <v>2</v>
+      </c>
+      <c r="E11" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>49</v>
+      </c>
+      <c r="B12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" t="s">
+        <v>54</v>
+      </c>
+      <c r="D12" t="s">
+        <v>2</v>
+      </c>
+      <c r="E12" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>58</v>
+      </c>
+      <c r="B13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" t="s">
+        <v>59</v>
+      </c>
+      <c r="D13" t="s">
+        <v>4</v>
+      </c>
+      <c r="E13" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>